<commit_message>
Reading Customer deatils from file added
</commit_message>
<xml_diff>
--- a/src/test/java/in/amazon/testData/LoginData.xlsx
+++ b/src/test/java/in/amazon/testData/LoginData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -32,20 +33,52 @@
   </si>
   <si>
     <t xml:space="preserve">bYsugyj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">411014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8421169991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password123*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pradeep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8421169992</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -67,6 +100,7 @@
       <color rgb="FF2A00FF"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,12 +145,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,68 +241,68 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -273,4 +315,83 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>